<commit_message>
fixing cancel count combinor
</commit_message>
<xml_diff>
--- a/excel_reports/David_Strehlow.xlsx
+++ b/excel_reports/David_Strehlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23295" uniqueCount="5052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23287" uniqueCount="5048">
   <si>
     <t>Policy Record</t>
   </si>
@@ -14594,22 +14594,10 @@
     <t>08-15-2021</t>
   </si>
   <si>
-    <t>3172447241</t>
-  </si>
-  <si>
-    <t>2737751</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Scalzo</t>
+    <t>3564371789</t>
   </si>
   <si>
     <t>10-28-2022</t>
-  </si>
-  <si>
-    <t>3564371789</t>
   </si>
   <si>
     <t>3564371852</t>
@@ -15589,12 +15577,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>5023</v>
+        <v>5019</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>5024</v>
+        <v>5020</v>
       </c>
       <c r="B2" s="2">
         <v>713</v>
@@ -15602,7 +15590,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>5025</v>
+        <v>5021</v>
       </c>
       <c r="B3" s="2">
         <v>951</v>
@@ -15610,18 +15598,18 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5026</v>
+        <v>5022</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5027</v>
+        <v>5023</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>5028</v>
+        <v>5024</v>
       </c>
       <c r="B5" s="4">
         <f>B3+B4-B2</f>
@@ -15630,7 +15618,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>5029</v>
+        <v>5025</v>
       </c>
       <c r="B6" s="2">
         <v>-30</v>
@@ -15638,30 +15626,30 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>5030</v>
+        <v>5026</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5031</v>
+        <v>5027</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>5032</v>
+        <v>5028</v>
       </c>
       <c r="B8" s="4">
         <f>SUM(B5:B7)</f>
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5033</v>
+        <v>5029</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>5034</v>
+        <v>5030</v>
       </c>
       <c r="B9" s="5">
         <f>MAX(0, B8*150)</f>
@@ -15670,12 +15658,12 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>5035</v>
+        <v>5031</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>5036</v>
+        <v>5032</v>
       </c>
       <c r="B12" s="2">
         <v>73</v>
@@ -15683,20 +15671,20 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>5037</v>
+        <v>5033</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>5038</v>
+        <v>5034</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5051</v>
+        <v>5047</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>5039</v>
+        <v>5035</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(Core!T:T)</f>
@@ -15705,12 +15693,12 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>5040</v>
+        <v>5036</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>5041</v>
+        <v>5037</v>
       </c>
       <c r="B20">
         <v>208</v>
@@ -15718,15 +15706,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>5042</v>
+        <v>5038</v>
       </c>
       <c r="B21">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>5043</v>
+        <v>5039</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
@@ -15734,7 +15722,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>5044</v>
+        <v>5040</v>
       </c>
       <c r="B23">
         <f>-B20+B21+B22</f>
@@ -15743,7 +15731,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>5045</v>
+        <v>5041</v>
       </c>
       <c r="B24" s="5">
         <f>B23*50</f>
@@ -15752,7 +15740,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>5046</v>
+        <v>5042</v>
       </c>
       <c r="B26">
         <v>9</v>
@@ -15760,7 +15748,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>5047</v>
+        <v>5043</v>
       </c>
       <c r="B27">
         <v>17</v>
@@ -15768,7 +15756,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>5048</v>
+        <v>5044</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -15776,7 +15764,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>5049</v>
+        <v>5045</v>
       </c>
       <c r="B29">
         <f>-B26+B27+B28</f>
@@ -15785,7 +15773,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>5050</v>
+        <v>5046</v>
       </c>
       <c r="B30" s="5">
         <f>B29*100</f>
@@ -18905,7 +18893,9 @@
       <c r="J7" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="K7" s="8"/>
+      <c r="K7" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="L7" s="8" t="s">
         <v>75</v>
       </c>
@@ -18942,7 +18932,9 @@
       <c r="J9" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="K9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="L9" s="8" t="s">
         <v>381</v>
       </c>
@@ -19020,7 +19012,9 @@
       <c r="J13" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="K13" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="L13" s="8" t="s">
         <v>75</v>
       </c>
@@ -27244,6 +27238,9 @@
       <c r="O262" t="s">
         <v>381</v>
       </c>
+      <c r="P262" t="s">
+        <v>130</v>
+      </c>
       <c r="Q262" s="8" t="s">
         <v>494</v>
       </c>
@@ -57025,6 +57022,9 @@
       <c r="O1377" t="s">
         <v>75</v>
       </c>
+      <c r="P1377" t="s">
+        <v>130</v>
+      </c>
       <c r="Q1377" s="8" t="s">
         <v>494</v>
       </c>
@@ -64549,6 +64549,9 @@
       </c>
       <c r="O1663" t="s">
         <v>75</v>
+      </c>
+      <c r="P1663" t="s">
+        <v>130</v>
       </c>
       <c r="Q1663" s="8" t="s">
         <v>494</v>
@@ -81817,7 +81820,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T508"/>
+  <dimension ref="A1:T506"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -88166,7 +88169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:14">
+    <row r="290" spans="1:16">
       <c r="A290" s="7" t="s">
         <v>4849</v>
       </c>
@@ -88210,7 +88213,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="292" spans="1:14">
+    <row r="292" spans="1:16">
       <c r="A292" s="7" t="s">
         <v>4850</v>
       </c>
@@ -88254,7 +88257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="294" spans="1:14">
+    <row r="294" spans="1:16">
       <c r="A294" s="7" t="s">
         <v>4851</v>
       </c>
@@ -88298,7 +88301,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="296" spans="1:14">
+    <row r="296" spans="1:16">
       <c r="A296" s="7" t="s">
         <v>4852</v>
       </c>
@@ -88339,7 +88342,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="298" spans="1:14">
+    <row r="298" spans="1:16">
       <c r="A298" s="7" t="s">
         <v>4853</v>
       </c>
@@ -88383,7 +88386,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="300" spans="1:14">
+    <row r="300" spans="1:16">
       <c r="A300" s="7" t="s">
         <v>4854</v>
       </c>
@@ -88427,15 +88430,15 @@
         <v>4856</v>
       </c>
     </row>
-    <row r="302" spans="1:14">
+    <row r="302" spans="1:16">
       <c r="A302" s="7" t="s">
         <v>4857</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>4858</v>
+        <v>2572</v>
       </c>
       <c r="C302" s="8" t="s">
-        <v>122</v>
+        <v>2573</v>
       </c>
       <c r="D302" s="8" t="s">
         <v>2574</v>
@@ -88447,17 +88450,14 @@
         <v>491</v>
       </c>
       <c r="G302" s="8" t="s">
-        <v>4859</v>
+        <v>30</v>
       </c>
       <c r="H302" s="8" t="s">
-        <v>4860</v>
+        <v>491</v>
       </c>
       <c r="I302" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J302" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K302" t="s">
         <v>4669</v>
       </c>
@@ -88465,15 +88465,59 @@
         <v>18</v>
       </c>
       <c r="M302" t="s">
-        <v>4861</v>
+        <v>4858</v>
       </c>
       <c r="N302" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="304" spans="1:14">
+    <row r="303" spans="1:16">
+      <c r="A303" s="7" t="s">
+        <v>4859</v>
+      </c>
+      <c r="B303" s="7" t="s">
+        <v>2572</v>
+      </c>
+      <c r="C303" s="8" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D303" s="8" t="s">
+        <v>2574</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F303" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="G303" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H303" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="I303" s="8" t="s">
+        <v>4668</v>
+      </c>
+      <c r="J303" s="8" t="s">
+        <v>4708</v>
+      </c>
+      <c r="K303" t="s">
+        <v>4669</v>
+      </c>
+      <c r="L303" t="s">
+        <v>1453</v>
+      </c>
+      <c r="M303" t="s">
+        <v>4858</v>
+      </c>
+      <c r="N303" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16">
       <c r="A304" s="7" t="s">
-        <v>4862</v>
+        <v>4860</v>
       </c>
       <c r="B304" s="7" t="s">
         <v>2572</v>
@@ -88499,75 +88543,37 @@
       <c r="I304" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J304" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K304" t="s">
         <v>4669</v>
       </c>
       <c r="L304" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M304" t="s">
-        <v>4861</v>
+        <v>326</v>
       </c>
       <c r="N304" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="305" spans="1:16">
-      <c r="A305" s="7" t="s">
-        <v>4863</v>
-      </c>
-      <c r="B305" s="7" t="s">
-        <v>2572</v>
-      </c>
-      <c r="C305" s="8" t="s">
-        <v>2573</v>
-      </c>
-      <c r="D305" s="8" t="s">
-        <v>2574</v>
-      </c>
-      <c r="E305" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F305" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="G305" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H305" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="I305" s="8" t="s">
-        <v>4668</v>
-      </c>
-      <c r="J305" s="8" t="s">
-        <v>4708</v>
-      </c>
-      <c r="K305" t="s">
-        <v>4669</v>
-      </c>
-      <c r="L305" t="s">
-        <v>1453</v>
-      </c>
-      <c r="M305" t="s">
+      <c r="P304" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14">
+      <c r="A306" s="7" t="s">
         <v>4861</v>
       </c>
-      <c r="N305" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="306" spans="1:16">
-      <c r="A306" s="7" t="s">
-        <v>4864</v>
-      </c>
       <c r="B306" s="7" t="s">
-        <v>2572</v>
+        <v>2580</v>
       </c>
       <c r="C306" s="8" t="s">
-        <v>2573</v>
+        <v>2581</v>
       </c>
       <c r="D306" s="8" t="s">
-        <v>2574</v>
+        <v>2582</v>
       </c>
       <c r="E306" s="8" t="s">
         <v>30</v>
@@ -88584,37 +88590,31 @@
       <c r="I306" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J306" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K306" t="s">
         <v>4669</v>
       </c>
       <c r="L306" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="M306" t="s">
-        <v>326</v>
+        <v>2990</v>
       </c>
       <c r="N306" t="s">
-        <v>35</v>
-      </c>
-      <c r="P306" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="308" spans="1:16">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14">
       <c r="A308" s="7" t="s">
-        <v>4865</v>
+        <v>4862</v>
       </c>
       <c r="B308" s="7" t="s">
-        <v>2580</v>
+        <v>2584</v>
       </c>
       <c r="C308" s="8" t="s">
-        <v>2581</v>
+        <v>2585</v>
       </c>
       <c r="D308" s="8" t="s">
-        <v>2582</v>
+        <v>2586</v>
       </c>
       <c r="E308" s="8" t="s">
         <v>30</v>
@@ -88631,6 +88631,9 @@
       <c r="I308" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J308" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K308" t="s">
         <v>4669</v>
       </c>
@@ -88638,24 +88641,24 @@
         <v>18</v>
       </c>
       <c r="M308" t="s">
-        <v>2990</v>
+        <v>672</v>
       </c>
       <c r="N308" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="310" spans="1:16">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14">
       <c r="A310" s="7" t="s">
-        <v>4866</v>
+        <v>4863</v>
       </c>
       <c r="B310" s="7" t="s">
-        <v>2584</v>
+        <v>2592</v>
       </c>
       <c r="C310" s="8" t="s">
-        <v>2585</v>
+        <v>2593</v>
       </c>
       <c r="D310" s="8" t="s">
-        <v>2586</v>
+        <v>2594</v>
       </c>
       <c r="E310" s="8" t="s">
         <v>30</v>
@@ -88672,9 +88675,6 @@
       <c r="I310" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J310" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K310" t="s">
         <v>4669</v>
       </c>
@@ -88682,24 +88682,24 @@
         <v>18</v>
       </c>
       <c r="M310" t="s">
-        <v>672</v>
+        <v>4864</v>
       </c>
       <c r="N310" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="312" spans="1:16">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14">
       <c r="A312" s="7" t="s">
-        <v>4867</v>
+        <v>4865</v>
       </c>
       <c r="B312" s="7" t="s">
-        <v>2592</v>
+        <v>2647</v>
       </c>
       <c r="C312" s="8" t="s">
-        <v>2593</v>
+        <v>136</v>
       </c>
       <c r="D312" s="8" t="s">
-        <v>2594</v>
+        <v>2648</v>
       </c>
       <c r="E312" s="8" t="s">
         <v>30</v>
@@ -88716,6 +88716,9 @@
       <c r="I312" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J312" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K312" t="s">
         <v>4669</v>
       </c>
@@ -88723,24 +88726,24 @@
         <v>18</v>
       </c>
       <c r="M312" t="s">
-        <v>4868</v>
+        <v>550</v>
       </c>
       <c r="N312" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="314" spans="1:16">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14">
       <c r="A314" s="7" t="s">
-        <v>4869</v>
+        <v>4866</v>
       </c>
       <c r="B314" s="7" t="s">
-        <v>2647</v>
+        <v>2688</v>
       </c>
       <c r="C314" s="8" t="s">
-        <v>136</v>
+        <v>2689</v>
       </c>
       <c r="D314" s="8" t="s">
-        <v>2648</v>
+        <v>2690</v>
       </c>
       <c r="E314" s="8" t="s">
         <v>30</v>
@@ -88757,9 +88760,6 @@
       <c r="I314" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J314" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K314" t="s">
         <v>4669</v>
       </c>
@@ -88767,21 +88767,21 @@
         <v>18</v>
       </c>
       <c r="M314" t="s">
-        <v>550</v>
+        <v>3710</v>
       </c>
       <c r="N314" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="316" spans="1:16">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14">
       <c r="A316" s="7" t="s">
-        <v>4870</v>
+        <v>4867</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>2688</v>
+        <v>2692</v>
       </c>
       <c r="C316" s="8" t="s">
-        <v>2689</v>
+        <v>2693</v>
       </c>
       <c r="D316" s="8" t="s">
         <v>2690</v>
@@ -88808,21 +88808,21 @@
         <v>18</v>
       </c>
       <c r="M316" t="s">
-        <v>3710</v>
+        <v>4868</v>
       </c>
       <c r="N316" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="318" spans="1:16">
+        <v>4869</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14">
       <c r="A318" s="7" t="s">
-        <v>4871</v>
+        <v>4870</v>
       </c>
       <c r="B318" s="7" t="s">
-        <v>2692</v>
+        <v>2696</v>
       </c>
       <c r="C318" s="8" t="s">
-        <v>2693</v>
+        <v>1293</v>
       </c>
       <c r="D318" s="8" t="s">
         <v>2690</v>
@@ -88849,24 +88849,24 @@
         <v>18</v>
       </c>
       <c r="M318" t="s">
-        <v>4872</v>
+        <v>1933</v>
       </c>
       <c r="N318" t="s">
-        <v>4873</v>
-      </c>
-    </row>
-    <row r="320" spans="1:16">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14">
       <c r="A320" s="7" t="s">
-        <v>4874</v>
+        <v>4871</v>
       </c>
       <c r="B320" s="7" t="s">
-        <v>2696</v>
+        <v>2722</v>
       </c>
       <c r="C320" s="8" t="s">
-        <v>1293</v>
+        <v>136</v>
       </c>
       <c r="D320" s="8" t="s">
-        <v>2690</v>
+        <v>2720</v>
       </c>
       <c r="E320" s="8" t="s">
         <v>30</v>
@@ -88883,6 +88883,9 @@
       <c r="I320" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J320" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K320" t="s">
         <v>4669</v>
       </c>
@@ -88890,24 +88893,24 @@
         <v>18</v>
       </c>
       <c r="M320" t="s">
-        <v>1933</v>
+        <v>325</v>
       </c>
       <c r="N320" t="s">
-        <v>405</v>
+        <v>27</v>
       </c>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="7" t="s">
-        <v>4875</v>
+        <v>4872</v>
       </c>
       <c r="B322" s="7" t="s">
-        <v>2722</v>
+        <v>2754</v>
       </c>
       <c r="C322" s="8" t="s">
-        <v>136</v>
+        <v>291</v>
       </c>
       <c r="D322" s="8" t="s">
-        <v>2720</v>
+        <v>2755</v>
       </c>
       <c r="E322" s="8" t="s">
         <v>30</v>
@@ -88934,21 +88937,21 @@
         <v>18</v>
       </c>
       <c r="M322" t="s">
-        <v>325</v>
+        <v>4873</v>
       </c>
       <c r="N322" t="s">
-        <v>27</v>
+        <v>427</v>
       </c>
     </row>
     <row r="324" spans="1:14">
       <c r="A324" s="7" t="s">
-        <v>4876</v>
+        <v>4874</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>2754</v>
+        <v>2758</v>
       </c>
       <c r="C324" s="8" t="s">
-        <v>291</v>
+        <v>204</v>
       </c>
       <c r="D324" s="8" t="s">
         <v>2755</v>
@@ -88968,9 +88971,6 @@
       <c r="I324" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J324" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K324" t="s">
         <v>4669</v>
       </c>
@@ -88978,24 +88978,24 @@
         <v>18</v>
       </c>
       <c r="M324" t="s">
-        <v>4877</v>
+        <v>1287</v>
       </c>
       <c r="N324" t="s">
-        <v>427</v>
+        <v>607</v>
       </c>
     </row>
     <row r="326" spans="1:14">
       <c r="A326" s="7" t="s">
-        <v>4878</v>
+        <v>4875</v>
       </c>
       <c r="B326" s="7" t="s">
-        <v>2758</v>
+        <v>2764</v>
       </c>
       <c r="C326" s="8" t="s">
-        <v>204</v>
+        <v>2765</v>
       </c>
       <c r="D326" s="8" t="s">
-        <v>2755</v>
+        <v>2766</v>
       </c>
       <c r="E326" s="8" t="s">
         <v>30</v>
@@ -89012,6 +89012,9 @@
       <c r="I326" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J326" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K326" t="s">
         <v>4669</v>
       </c>
@@ -89019,24 +89022,24 @@
         <v>18</v>
       </c>
       <c r="M326" t="s">
-        <v>1287</v>
+        <v>1715</v>
       </c>
       <c r="N326" t="s">
-        <v>607</v>
+        <v>427</v>
       </c>
     </row>
     <row r="328" spans="1:14">
       <c r="A328" s="7" t="s">
-        <v>4879</v>
+        <v>4876</v>
       </c>
       <c r="B328" s="7" t="s">
-        <v>2764</v>
+        <v>2773</v>
       </c>
       <c r="C328" s="8" t="s">
-        <v>2765</v>
+        <v>2774</v>
       </c>
       <c r="D328" s="8" t="s">
-        <v>2766</v>
+        <v>2775</v>
       </c>
       <c r="E328" s="8" t="s">
         <v>30</v>
@@ -89063,24 +89066,24 @@
         <v>18</v>
       </c>
       <c r="M328" t="s">
-        <v>1715</v>
+        <v>1339</v>
       </c>
       <c r="N328" t="s">
-        <v>427</v>
+        <v>591</v>
       </c>
     </row>
     <row r="330" spans="1:14">
       <c r="A330" s="7" t="s">
-        <v>4880</v>
+        <v>4877</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>2773</v>
+        <v>2785</v>
       </c>
       <c r="C330" s="8" t="s">
-        <v>2774</v>
+        <v>30</v>
       </c>
       <c r="D330" s="8" t="s">
-        <v>2775</v>
+        <v>2786</v>
       </c>
       <c r="E330" s="8" t="s">
         <v>30</v>
@@ -89107,24 +89110,24 @@
         <v>18</v>
       </c>
       <c r="M330" t="s">
-        <v>1339</v>
+        <v>2787</v>
       </c>
       <c r="N330" t="s">
-        <v>591</v>
+        <v>405</v>
       </c>
     </row>
     <row r="332" spans="1:14">
       <c r="A332" s="7" t="s">
-        <v>4881</v>
+        <v>4878</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>2785</v>
+        <v>2789</v>
       </c>
       <c r="C332" s="8" t="s">
-        <v>30</v>
+        <v>408</v>
       </c>
       <c r="D332" s="8" t="s">
-        <v>2786</v>
+        <v>2790</v>
       </c>
       <c r="E332" s="8" t="s">
         <v>30</v>
@@ -89151,24 +89154,24 @@
         <v>18</v>
       </c>
       <c r="M332" t="s">
-        <v>2787</v>
+        <v>667</v>
       </c>
       <c r="N332" t="s">
-        <v>405</v>
+        <v>200</v>
       </c>
     </row>
     <row r="334" spans="1:14">
       <c r="A334" s="7" t="s">
-        <v>4882</v>
+        <v>4879</v>
       </c>
       <c r="B334" s="7" t="s">
-        <v>2789</v>
+        <v>2792</v>
       </c>
       <c r="C334" s="8" t="s">
-        <v>408</v>
+        <v>2793</v>
       </c>
       <c r="D334" s="8" t="s">
-        <v>2790</v>
+        <v>2794</v>
       </c>
       <c r="E334" s="8" t="s">
         <v>30</v>
@@ -89185,9 +89188,6 @@
       <c r="I334" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J334" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K334" t="s">
         <v>4669</v>
       </c>
@@ -89195,24 +89195,24 @@
         <v>18</v>
       </c>
       <c r="M334" t="s">
-        <v>667</v>
+        <v>4657</v>
       </c>
       <c r="N334" t="s">
-        <v>200</v>
+        <v>596</v>
       </c>
     </row>
     <row r="336" spans="1:14">
       <c r="A336" s="7" t="s">
-        <v>4883</v>
+        <v>4880</v>
       </c>
       <c r="B336" s="7" t="s">
-        <v>2792</v>
+        <v>2803</v>
       </c>
       <c r="C336" s="8" t="s">
-        <v>2793</v>
+        <v>166</v>
       </c>
       <c r="D336" s="8" t="s">
-        <v>2794</v>
+        <v>2804</v>
       </c>
       <c r="E336" s="8" t="s">
         <v>30</v>
@@ -89236,24 +89236,24 @@
         <v>18</v>
       </c>
       <c r="M336" t="s">
-        <v>4657</v>
+        <v>4683</v>
       </c>
       <c r="N336" t="s">
-        <v>596</v>
+        <v>365</v>
       </c>
     </row>
     <row r="338" spans="1:14">
       <c r="A338" s="7" t="s">
-        <v>4884</v>
+        <v>4881</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>2803</v>
+        <v>2827</v>
       </c>
       <c r="C338" s="8" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="D338" s="8" t="s">
-        <v>2804</v>
+        <v>2825</v>
       </c>
       <c r="E338" s="8" t="s">
         <v>30</v>
@@ -89277,24 +89277,24 @@
         <v>18</v>
       </c>
       <c r="M338" t="s">
-        <v>4683</v>
+        <v>769</v>
       </c>
       <c r="N338" t="s">
-        <v>365</v>
+        <v>607</v>
       </c>
     </row>
     <row r="340" spans="1:14">
       <c r="A340" s="7" t="s">
-        <v>4885</v>
+        <v>4882</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>2827</v>
+        <v>2845</v>
       </c>
       <c r="C340" s="8" t="s">
-        <v>30</v>
+        <v>2846</v>
       </c>
       <c r="D340" s="8" t="s">
-        <v>2825</v>
+        <v>2847</v>
       </c>
       <c r="E340" s="8" t="s">
         <v>30</v>
@@ -89311,6 +89311,9 @@
       <c r="I340" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J340" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K340" t="s">
         <v>4669</v>
       </c>
@@ -89318,21 +89321,21 @@
         <v>18</v>
       </c>
       <c r="M340" t="s">
-        <v>769</v>
+        <v>2848</v>
       </c>
       <c r="N340" t="s">
-        <v>607</v>
+        <v>395</v>
       </c>
     </row>
     <row r="342" spans="1:14">
       <c r="A342" s="7" t="s">
-        <v>4886</v>
+        <v>4883</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>2845</v>
+        <v>4884</v>
       </c>
       <c r="C342" s="8" t="s">
-        <v>2846</v>
+        <v>4885</v>
       </c>
       <c r="D342" s="8" t="s">
         <v>2847</v>
@@ -89370,16 +89373,16 @@
     </row>
     <row r="344" spans="1:14">
       <c r="A344" s="7" t="s">
-        <v>4887</v>
+        <v>4886</v>
       </c>
       <c r="B344" s="7" t="s">
-        <v>4888</v>
+        <v>2854</v>
       </c>
       <c r="C344" s="8" t="s">
-        <v>4889</v>
+        <v>1181</v>
       </c>
       <c r="D344" s="8" t="s">
-        <v>2847</v>
+        <v>2855</v>
       </c>
       <c r="E344" s="8" t="s">
         <v>30</v>
@@ -89406,24 +89409,24 @@
         <v>18</v>
       </c>
       <c r="M344" t="s">
-        <v>2848</v>
+        <v>2578</v>
       </c>
       <c r="N344" t="s">
-        <v>395</v>
+        <v>596</v>
       </c>
     </row>
     <row r="346" spans="1:14">
       <c r="A346" s="7" t="s">
-        <v>4890</v>
+        <v>4887</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>2854</v>
+        <v>2869</v>
       </c>
       <c r="C346" s="8" t="s">
-        <v>1181</v>
+        <v>767</v>
       </c>
       <c r="D346" s="8" t="s">
-        <v>2855</v>
+        <v>2870</v>
       </c>
       <c r="E346" s="8" t="s">
         <v>30</v>
@@ -89450,24 +89453,24 @@
         <v>18</v>
       </c>
       <c r="M346" t="s">
-        <v>2578</v>
+        <v>2122</v>
       </c>
       <c r="N346" t="s">
-        <v>596</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="348" spans="1:14">
       <c r="A348" s="7" t="s">
-        <v>4891</v>
+        <v>4888</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>2869</v>
+        <v>2881</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>767</v>
+        <v>2882</v>
       </c>
       <c r="D348" s="8" t="s">
-        <v>2870</v>
+        <v>2883</v>
       </c>
       <c r="E348" s="8" t="s">
         <v>30</v>
@@ -89494,24 +89497,24 @@
         <v>18</v>
       </c>
       <c r="M348" t="s">
-        <v>2122</v>
+        <v>34</v>
       </c>
       <c r="N348" t="s">
-        <v>1063</v>
+        <v>74</v>
       </c>
     </row>
     <row r="350" spans="1:14">
       <c r="A350" s="7" t="s">
-        <v>4892</v>
+        <v>4889</v>
       </c>
       <c r="B350" s="7" t="s">
-        <v>2881</v>
+        <v>2891</v>
       </c>
       <c r="C350" s="8" t="s">
-        <v>2882</v>
+        <v>2892</v>
       </c>
       <c r="D350" s="8" t="s">
-        <v>2883</v>
+        <v>2887</v>
       </c>
       <c r="E350" s="8" t="s">
         <v>30</v>
@@ -89529,7 +89532,7 @@
         <v>4668</v>
       </c>
       <c r="J350" s="8" t="s">
-        <v>4671</v>
+        <v>4708</v>
       </c>
       <c r="K350" t="s">
         <v>4669</v>
@@ -89538,21 +89541,21 @@
         <v>18</v>
       </c>
       <c r="M350" t="s">
-        <v>34</v>
+        <v>3581</v>
       </c>
       <c r="N350" t="s">
-        <v>74</v>
+        <v>859</v>
       </c>
     </row>
     <row r="352" spans="1:14">
       <c r="A352" s="7" t="s">
-        <v>4893</v>
+        <v>4890</v>
       </c>
       <c r="B352" s="7" t="s">
-        <v>2891</v>
+        <v>4891</v>
       </c>
       <c r="C352" s="8" t="s">
-        <v>2892</v>
+        <v>1713</v>
       </c>
       <c r="D352" s="8" t="s">
         <v>2887</v>
@@ -89572,9 +89575,6 @@
       <c r="I352" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J352" s="8" t="s">
-        <v>4708</v>
-      </c>
       <c r="K352" t="s">
         <v>4669</v>
       </c>
@@ -89590,13 +89590,13 @@
     </row>
     <row r="354" spans="1:16">
       <c r="A354" s="7" t="s">
-        <v>4894</v>
+        <v>4892</v>
       </c>
       <c r="B354" s="7" t="s">
-        <v>4895</v>
+        <v>2889</v>
       </c>
       <c r="C354" s="8" t="s">
-        <v>1713</v>
+        <v>1472</v>
       </c>
       <c r="D354" s="8" t="s">
         <v>2887</v>
@@ -89616,6 +89616,9 @@
       <c r="I354" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J354" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K354" t="s">
         <v>4669</v>
       </c>
@@ -89623,24 +89626,24 @@
         <v>18</v>
       </c>
       <c r="M354" t="s">
-        <v>3581</v>
+        <v>2638</v>
       </c>
       <c r="N354" t="s">
-        <v>859</v>
+        <v>405</v>
       </c>
     </row>
     <row r="356" spans="1:16">
       <c r="A356" s="7" t="s">
-        <v>4896</v>
+        <v>4893</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>2889</v>
+        <v>2905</v>
       </c>
       <c r="C356" s="8" t="s">
-        <v>1472</v>
+        <v>2906</v>
       </c>
       <c r="D356" s="8" t="s">
-        <v>2887</v>
+        <v>2851</v>
       </c>
       <c r="E356" s="8" t="s">
         <v>30</v>
@@ -89667,24 +89670,24 @@
         <v>18</v>
       </c>
       <c r="M356" t="s">
-        <v>2638</v>
+        <v>55</v>
       </c>
       <c r="N356" t="s">
-        <v>405</v>
+        <v>35</v>
       </c>
     </row>
     <row r="358" spans="1:16">
       <c r="A358" s="7" t="s">
-        <v>4897</v>
+        <v>4894</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>2905</v>
+        <v>2918</v>
       </c>
       <c r="C358" s="8" t="s">
-        <v>2906</v>
+        <v>610</v>
       </c>
       <c r="D358" s="8" t="s">
-        <v>2851</v>
+        <v>2919</v>
       </c>
       <c r="E358" s="8" t="s">
         <v>30</v>
@@ -89711,7 +89714,7 @@
         <v>18</v>
       </c>
       <c r="M358" t="s">
-        <v>55</v>
+        <v>2875</v>
       </c>
       <c r="N358" t="s">
         <v>35</v>
@@ -89719,16 +89722,16 @@
     </row>
     <row r="360" spans="1:16">
       <c r="A360" s="7" t="s">
-        <v>4898</v>
+        <v>4895</v>
       </c>
       <c r="B360" s="7" t="s">
-        <v>2918</v>
+        <v>2925</v>
       </c>
       <c r="C360" s="8" t="s">
-        <v>610</v>
+        <v>1806</v>
       </c>
       <c r="D360" s="8" t="s">
-        <v>2919</v>
+        <v>2926</v>
       </c>
       <c r="E360" s="8" t="s">
         <v>30</v>
@@ -89755,24 +89758,24 @@
         <v>18</v>
       </c>
       <c r="M360" t="s">
-        <v>2875</v>
+        <v>2227</v>
       </c>
       <c r="N360" t="s">
-        <v>35</v>
+        <v>412</v>
       </c>
     </row>
     <row r="362" spans="1:16">
       <c r="A362" s="7" t="s">
-        <v>4899</v>
+        <v>4896</v>
       </c>
       <c r="B362" s="7" t="s">
-        <v>2925</v>
+        <v>2940</v>
       </c>
       <c r="C362" s="8" t="s">
-        <v>1806</v>
+        <v>291</v>
       </c>
       <c r="D362" s="8" t="s">
-        <v>2926</v>
+        <v>2938</v>
       </c>
       <c r="E362" s="8" t="s">
         <v>30</v>
@@ -89796,24 +89799,30 @@
         <v>4669</v>
       </c>
       <c r="L362" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="M362" t="s">
-        <v>2227</v>
+        <v>681</v>
       </c>
       <c r="N362" t="s">
-        <v>412</v>
+        <v>2605</v>
+      </c>
+      <c r="O362" t="s">
+        <v>1051</v>
+      </c>
+      <c r="P362" t="s">
+        <v>1051</v>
       </c>
     </row>
     <row r="364" spans="1:16">
       <c r="A364" s="7" t="s">
-        <v>4900</v>
+        <v>4897</v>
       </c>
       <c r="B364" s="7" t="s">
-        <v>2940</v>
+        <v>2937</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="D364" s="8" t="s">
         <v>2938</v>
@@ -89833,40 +89842,31 @@
       <c r="I364" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J364" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K364" t="s">
         <v>4669</v>
       </c>
       <c r="L364" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="M364" t="s">
-        <v>681</v>
+        <v>2412</v>
       </c>
       <c r="N364" t="s">
-        <v>2605</v>
-      </c>
-      <c r="O364" t="s">
-        <v>1051</v>
-      </c>
-      <c r="P364" t="s">
-        <v>1051</v>
+        <v>651</v>
       </c>
     </row>
     <row r="366" spans="1:16">
       <c r="A366" s="7" t="s">
-        <v>4901</v>
+        <v>4898</v>
       </c>
       <c r="B366" s="7" t="s">
-        <v>2937</v>
+        <v>2978</v>
       </c>
       <c r="C366" s="8" t="s">
-        <v>277</v>
+        <v>1406</v>
       </c>
       <c r="D366" s="8" t="s">
-        <v>2938</v>
+        <v>2979</v>
       </c>
       <c r="E366" s="8" t="s">
         <v>30</v>
@@ -89883,6 +89883,9 @@
       <c r="I366" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J366" s="8" t="s">
+        <v>4708</v>
+      </c>
       <c r="K366" t="s">
         <v>4669</v>
       </c>
@@ -89890,24 +89893,24 @@
         <v>18</v>
       </c>
       <c r="M366" t="s">
-        <v>2412</v>
+        <v>2980</v>
       </c>
       <c r="N366" t="s">
-        <v>651</v>
+        <v>405</v>
       </c>
     </row>
     <row r="368" spans="1:16">
       <c r="A368" s="7" t="s">
-        <v>4902</v>
+        <v>4899</v>
       </c>
       <c r="B368" s="7" t="s">
-        <v>2978</v>
+        <v>2992</v>
       </c>
       <c r="C368" s="8" t="s">
-        <v>1406</v>
+        <v>2993</v>
       </c>
       <c r="D368" s="8" t="s">
-        <v>2979</v>
+        <v>2994</v>
       </c>
       <c r="E368" s="8" t="s">
         <v>30</v>
@@ -89925,7 +89928,7 @@
         <v>4668</v>
       </c>
       <c r="J368" s="8" t="s">
-        <v>4708</v>
+        <v>4671</v>
       </c>
       <c r="K368" t="s">
         <v>4669</v>
@@ -89934,24 +89937,24 @@
         <v>18</v>
       </c>
       <c r="M368" t="s">
-        <v>2980</v>
+        <v>2995</v>
       </c>
       <c r="N368" t="s">
-        <v>405</v>
+        <v>551</v>
       </c>
     </row>
     <row r="370" spans="1:16">
       <c r="A370" s="7" t="s">
-        <v>4903</v>
+        <v>4900</v>
       </c>
       <c r="B370" s="7" t="s">
-        <v>2992</v>
+        <v>3012</v>
       </c>
       <c r="C370" s="8" t="s">
-        <v>2993</v>
+        <v>723</v>
       </c>
       <c r="D370" s="8" t="s">
-        <v>2994</v>
+        <v>2400</v>
       </c>
       <c r="E370" s="8" t="s">
         <v>30</v>
@@ -89968,34 +89971,37 @@
       <c r="I370" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J370" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K370" t="s">
         <v>4669</v>
       </c>
       <c r="L370" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="M370" t="s">
-        <v>2995</v>
+        <v>1191</v>
       </c>
       <c r="N370" t="s">
-        <v>551</v>
+        <v>412</v>
+      </c>
+      <c r="O370" t="s">
+        <v>1051</v>
+      </c>
+      <c r="P370" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="372" spans="1:16">
       <c r="A372" s="7" t="s">
-        <v>4904</v>
+        <v>4901</v>
       </c>
       <c r="B372" s="7" t="s">
-        <v>3012</v>
+        <v>3024</v>
       </c>
       <c r="C372" s="8" t="s">
-        <v>723</v>
+        <v>61</v>
       </c>
       <c r="D372" s="8" t="s">
-        <v>2400</v>
+        <v>3025</v>
       </c>
       <c r="E372" s="8" t="s">
         <v>30</v>
@@ -90012,37 +90018,34 @@
       <c r="I372" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J372" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K372" t="s">
         <v>4669</v>
       </c>
       <c r="L372" t="s">
-        <v>72</v>
+        <v>1453</v>
       </c>
       <c r="M372" t="s">
-        <v>1191</v>
+        <v>247</v>
       </c>
       <c r="N372" t="s">
-        <v>412</v>
-      </c>
-      <c r="O372" t="s">
-        <v>1051</v>
-      </c>
-      <c r="P372" t="s">
-        <v>358</v>
+        <v>74</v>
       </c>
     </row>
     <row r="374" spans="1:16">
       <c r="A374" s="7" t="s">
-        <v>4905</v>
+        <v>4902</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>3024</v>
+        <v>3031</v>
       </c>
       <c r="C374" s="8" t="s">
-        <v>61</v>
+        <v>3032</v>
       </c>
       <c r="D374" s="8" t="s">
-        <v>3025</v>
+        <v>3033</v>
       </c>
       <c r="E374" s="8" t="s">
         <v>30</v>
@@ -90059,34 +90062,31 @@
       <c r="I374" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J374" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K374" t="s">
         <v>4669</v>
       </c>
       <c r="L374" t="s">
-        <v>1453</v>
+        <v>18</v>
       </c>
       <c r="M374" t="s">
-        <v>247</v>
+        <v>1621</v>
       </c>
       <c r="N374" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
     </row>
     <row r="376" spans="1:16">
       <c r="A376" s="7" t="s">
-        <v>4906</v>
+        <v>4903</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>3031</v>
+        <v>3038</v>
       </c>
       <c r="C376" s="8" t="s">
-        <v>3032</v>
+        <v>3039</v>
       </c>
       <c r="D376" s="8" t="s">
-        <v>3033</v>
+        <v>3040</v>
       </c>
       <c r="E376" s="8" t="s">
         <v>30</v>
@@ -90103,6 +90103,9 @@
       <c r="I376" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J376" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K376" t="s">
         <v>4669</v>
       </c>
@@ -90110,24 +90113,24 @@
         <v>18</v>
       </c>
       <c r="M376" t="s">
-        <v>1621</v>
+        <v>1251</v>
       </c>
       <c r="N376" t="s">
-        <v>27</v>
+        <v>493</v>
       </c>
     </row>
     <row r="378" spans="1:16">
       <c r="A378" s="7" t="s">
-        <v>4907</v>
+        <v>4904</v>
       </c>
       <c r="B378" s="7" t="s">
-        <v>3038</v>
+        <v>3042</v>
       </c>
       <c r="C378" s="8" t="s">
-        <v>3039</v>
+        <v>3043</v>
       </c>
       <c r="D378" s="8" t="s">
-        <v>3040</v>
+        <v>3044</v>
       </c>
       <c r="E378" s="8" t="s">
         <v>30</v>
@@ -90144,9 +90147,6 @@
       <c r="I378" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J378" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K378" t="s">
         <v>4669</v>
       </c>
@@ -90154,24 +90154,24 @@
         <v>18</v>
       </c>
       <c r="M378" t="s">
-        <v>1251</v>
+        <v>1891</v>
       </c>
       <c r="N378" t="s">
-        <v>493</v>
+        <v>380</v>
       </c>
     </row>
     <row r="380" spans="1:16">
       <c r="A380" s="7" t="s">
-        <v>4908</v>
+        <v>4905</v>
       </c>
       <c r="B380" s="7" t="s">
-        <v>3042</v>
+        <v>3057</v>
       </c>
       <c r="C380" s="8" t="s">
-        <v>3043</v>
+        <v>3058</v>
       </c>
       <c r="D380" s="8" t="s">
-        <v>3044</v>
+        <v>3055</v>
       </c>
       <c r="E380" s="8" t="s">
         <v>30</v>
@@ -90188,6 +90188,9 @@
       <c r="I380" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J380" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K380" t="s">
         <v>4669</v>
       </c>
@@ -90195,24 +90198,24 @@
         <v>18</v>
       </c>
       <c r="M380" t="s">
-        <v>1891</v>
+        <v>974</v>
       </c>
       <c r="N380" t="s">
-        <v>380</v>
+        <v>551</v>
       </c>
     </row>
     <row r="382" spans="1:16">
       <c r="A382" s="7" t="s">
-        <v>4909</v>
+        <v>4906</v>
       </c>
       <c r="B382" s="7" t="s">
-        <v>3057</v>
+        <v>3072</v>
       </c>
       <c r="C382" s="8" t="s">
-        <v>3058</v>
+        <v>3073</v>
       </c>
       <c r="D382" s="8" t="s">
-        <v>3055</v>
+        <v>3070</v>
       </c>
       <c r="E382" s="8" t="s">
         <v>30</v>
@@ -90239,21 +90242,21 @@
         <v>18</v>
       </c>
       <c r="M382" t="s">
-        <v>974</v>
+        <v>788</v>
       </c>
       <c r="N382" t="s">
-        <v>551</v>
+        <v>27</v>
       </c>
     </row>
     <row r="384" spans="1:16">
       <c r="A384" s="7" t="s">
-        <v>4910</v>
+        <v>4907</v>
       </c>
       <c r="B384" s="7" t="s">
-        <v>3072</v>
+        <v>3068</v>
       </c>
       <c r="C384" s="8" t="s">
-        <v>3073</v>
+        <v>3069</v>
       </c>
       <c r="D384" s="8" t="s">
         <v>3070</v>
@@ -90283,24 +90286,24 @@
         <v>18</v>
       </c>
       <c r="M384" t="s">
-        <v>788</v>
+        <v>2304</v>
       </c>
       <c r="N384" t="s">
-        <v>27</v>
+        <v>254</v>
       </c>
     </row>
     <row r="386" spans="1:14">
       <c r="A386" s="7" t="s">
-        <v>4911</v>
+        <v>4908</v>
       </c>
       <c r="B386" s="7" t="s">
-        <v>3068</v>
+        <v>3088</v>
       </c>
       <c r="C386" s="8" t="s">
-        <v>3069</v>
+        <v>3089</v>
       </c>
       <c r="D386" s="8" t="s">
-        <v>3070</v>
+        <v>3090</v>
       </c>
       <c r="E386" s="8" t="s">
         <v>30</v>
@@ -90317,9 +90320,6 @@
       <c r="I386" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J386" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K386" t="s">
         <v>4669</v>
       </c>
@@ -90327,24 +90327,24 @@
         <v>18</v>
       </c>
       <c r="M386" t="s">
-        <v>2304</v>
+        <v>4909</v>
       </c>
       <c r="N386" t="s">
-        <v>254</v>
+        <v>527</v>
       </c>
     </row>
     <row r="388" spans="1:14">
       <c r="A388" s="7" t="s">
-        <v>4912</v>
+        <v>4910</v>
       </c>
       <c r="B388" s="7" t="s">
-        <v>3088</v>
+        <v>3109</v>
       </c>
       <c r="C388" s="8" t="s">
-        <v>3089</v>
+        <v>170</v>
       </c>
       <c r="D388" s="8" t="s">
-        <v>3090</v>
+        <v>3107</v>
       </c>
       <c r="E388" s="8" t="s">
         <v>30</v>
@@ -90361,6 +90361,9 @@
       <c r="I388" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J388" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K388" t="s">
         <v>4669</v>
       </c>
@@ -90368,21 +90371,21 @@
         <v>18</v>
       </c>
       <c r="M388" t="s">
-        <v>4913</v>
+        <v>1857</v>
       </c>
       <c r="N388" t="s">
-        <v>527</v>
+        <v>405</v>
       </c>
     </row>
     <row r="390" spans="1:14">
       <c r="A390" s="7" t="s">
-        <v>4914</v>
+        <v>4911</v>
       </c>
       <c r="B390" s="7" t="s">
-        <v>3109</v>
+        <v>3105</v>
       </c>
       <c r="C390" s="8" t="s">
-        <v>170</v>
+        <v>3106</v>
       </c>
       <c r="D390" s="8" t="s">
         <v>3107</v>
@@ -90412,7 +90415,7 @@
         <v>18</v>
       </c>
       <c r="M390" t="s">
-        <v>1857</v>
+        <v>404</v>
       </c>
       <c r="N390" t="s">
         <v>405</v>
@@ -90420,16 +90423,16 @@
     </row>
     <row r="392" spans="1:14">
       <c r="A392" s="7" t="s">
-        <v>4915</v>
+        <v>4912</v>
       </c>
       <c r="B392" s="7" t="s">
-        <v>3105</v>
+        <v>3125</v>
       </c>
       <c r="C392" s="8" t="s">
-        <v>3106</v>
+        <v>3126</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>3107</v>
+        <v>3127</v>
       </c>
       <c r="E392" s="8" t="s">
         <v>30</v>
@@ -90456,21 +90459,21 @@
         <v>18</v>
       </c>
       <c r="M392" t="s">
-        <v>404</v>
+        <v>3240</v>
       </c>
       <c r="N392" t="s">
-        <v>405</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="394" spans="1:14">
       <c r="A394" s="7" t="s">
-        <v>4916</v>
+        <v>4913</v>
       </c>
       <c r="B394" s="7" t="s">
-        <v>3125</v>
+        <v>3129</v>
       </c>
       <c r="C394" s="8" t="s">
-        <v>3126</v>
+        <v>391</v>
       </c>
       <c r="D394" s="8" t="s">
         <v>3127</v>
@@ -90508,16 +90511,16 @@
     </row>
     <row r="396" spans="1:14">
       <c r="A396" s="7" t="s">
-        <v>4917</v>
+        <v>4914</v>
       </c>
       <c r="B396" s="7" t="s">
-        <v>3129</v>
+        <v>3150</v>
       </c>
       <c r="C396" s="8" t="s">
-        <v>391</v>
+        <v>2165</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>3127</v>
+        <v>3151</v>
       </c>
       <c r="E396" s="8" t="s">
         <v>30</v>
@@ -90534,9 +90537,6 @@
       <c r="I396" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J396" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K396" t="s">
         <v>4669</v>
       </c>
@@ -90544,24 +90544,24 @@
         <v>18</v>
       </c>
       <c r="M396" t="s">
-        <v>3240</v>
+        <v>643</v>
       </c>
       <c r="N396" t="s">
-        <v>3241</v>
+        <v>601</v>
       </c>
     </row>
     <row r="398" spans="1:14">
       <c r="A398" s="7" t="s">
-        <v>4918</v>
+        <v>4915</v>
       </c>
       <c r="B398" s="7" t="s">
-        <v>3150</v>
+        <v>3154</v>
       </c>
       <c r="C398" s="8" t="s">
-        <v>2165</v>
+        <v>2929</v>
       </c>
       <c r="D398" s="8" t="s">
-        <v>3151</v>
+        <v>3155</v>
       </c>
       <c r="E398" s="8" t="s">
         <v>30</v>
@@ -90578,6 +90578,9 @@
       <c r="I398" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J398" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K398" t="s">
         <v>4669</v>
       </c>
@@ -90585,21 +90588,21 @@
         <v>18</v>
       </c>
       <c r="M398" t="s">
-        <v>643</v>
+        <v>3269</v>
       </c>
       <c r="N398" t="s">
-        <v>601</v>
+        <v>412</v>
       </c>
     </row>
     <row r="400" spans="1:14">
       <c r="A400" s="7" t="s">
-        <v>4919</v>
+        <v>4916</v>
       </c>
       <c r="B400" s="7" t="s">
-        <v>3154</v>
+        <v>4917</v>
       </c>
       <c r="C400" s="8" t="s">
-        <v>2929</v>
+        <v>4918</v>
       </c>
       <c r="D400" s="8" t="s">
         <v>3155</v>
@@ -90637,16 +90640,16 @@
     </row>
     <row r="402" spans="1:14">
       <c r="A402" s="7" t="s">
-        <v>4920</v>
+        <v>4919</v>
       </c>
       <c r="B402" s="7" t="s">
-        <v>4921</v>
+        <v>3168</v>
       </c>
       <c r="C402" s="8" t="s">
-        <v>4922</v>
+        <v>277</v>
       </c>
       <c r="D402" s="8" t="s">
-        <v>3155</v>
+        <v>3169</v>
       </c>
       <c r="E402" s="8" t="s">
         <v>30</v>
@@ -90673,7 +90676,7 @@
         <v>18</v>
       </c>
       <c r="M402" t="s">
-        <v>3269</v>
+        <v>2184</v>
       </c>
       <c r="N402" t="s">
         <v>412</v>
@@ -90681,16 +90684,16 @@
     </row>
     <row r="404" spans="1:14">
       <c r="A404" s="7" t="s">
-        <v>4923</v>
+        <v>4920</v>
       </c>
       <c r="B404" s="7" t="s">
-        <v>3168</v>
+        <v>3178</v>
       </c>
       <c r="C404" s="8" t="s">
-        <v>277</v>
+        <v>65</v>
       </c>
       <c r="D404" s="8" t="s">
-        <v>3169</v>
+        <v>3179</v>
       </c>
       <c r="E404" s="8" t="s">
         <v>30</v>
@@ -90714,27 +90717,27 @@
         <v>4669</v>
       </c>
       <c r="L404" t="s">
-        <v>18</v>
+        <v>1453</v>
       </c>
       <c r="M404" t="s">
-        <v>2184</v>
+        <v>468</v>
       </c>
       <c r="N404" t="s">
-        <v>412</v>
+        <v>21</v>
       </c>
     </row>
     <row r="406" spans="1:14">
       <c r="A406" s="7" t="s">
-        <v>4924</v>
+        <v>4921</v>
       </c>
       <c r="B406" s="7" t="s">
-        <v>3178</v>
+        <v>3190</v>
       </c>
       <c r="C406" s="8" t="s">
-        <v>65</v>
+        <v>712</v>
       </c>
       <c r="D406" s="8" t="s">
-        <v>3179</v>
+        <v>3191</v>
       </c>
       <c r="E406" s="8" t="s">
         <v>30</v>
@@ -90751,34 +90754,31 @@
       <c r="I406" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J406" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K406" t="s">
         <v>4669</v>
       </c>
       <c r="L406" t="s">
-        <v>1453</v>
+        <v>18</v>
       </c>
       <c r="M406" t="s">
-        <v>468</v>
+        <v>3192</v>
       </c>
       <c r="N406" t="s">
-        <v>21</v>
+        <v>365</v>
       </c>
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="7" t="s">
-        <v>4925</v>
+        <v>4922</v>
       </c>
       <c r="B408" s="7" t="s">
-        <v>3190</v>
+        <v>3203</v>
       </c>
       <c r="C408" s="8" t="s">
-        <v>712</v>
+        <v>3204</v>
       </c>
       <c r="D408" s="8" t="s">
-        <v>3191</v>
+        <v>3205</v>
       </c>
       <c r="E408" s="8" t="s">
         <v>30</v>
@@ -90802,24 +90802,24 @@
         <v>18</v>
       </c>
       <c r="M408" t="s">
-        <v>3192</v>
+        <v>1698</v>
       </c>
       <c r="N408" t="s">
-        <v>365</v>
+        <v>254</v>
       </c>
     </row>
     <row r="410" spans="1:14">
       <c r="A410" s="7" t="s">
-        <v>4926</v>
+        <v>4923</v>
       </c>
       <c r="B410" s="7" t="s">
-        <v>3203</v>
+        <v>3207</v>
       </c>
       <c r="C410" s="8" t="s">
-        <v>3204</v>
+        <v>3208</v>
       </c>
       <c r="D410" s="8" t="s">
-        <v>3205</v>
+        <v>3209</v>
       </c>
       <c r="E410" s="8" t="s">
         <v>30</v>
@@ -90836,6 +90836,9 @@
       <c r="I410" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J410" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K410" t="s">
         <v>4669</v>
       </c>
@@ -90843,24 +90846,24 @@
         <v>18</v>
       </c>
       <c r="M410" t="s">
-        <v>1698</v>
+        <v>1042</v>
       </c>
       <c r="N410" t="s">
-        <v>254</v>
+        <v>427</v>
       </c>
     </row>
     <row r="412" spans="1:14">
       <c r="A412" s="7" t="s">
-        <v>4927</v>
+        <v>4924</v>
       </c>
       <c r="B412" s="7" t="s">
-        <v>3207</v>
+        <v>3227</v>
       </c>
       <c r="C412" s="8" t="s">
-        <v>3208</v>
+        <v>3228</v>
       </c>
       <c r="D412" s="8" t="s">
-        <v>3209</v>
+        <v>3229</v>
       </c>
       <c r="E412" s="8" t="s">
         <v>30</v>
@@ -90887,24 +90890,24 @@
         <v>18</v>
       </c>
       <c r="M412" t="s">
-        <v>1042</v>
+        <v>4925</v>
       </c>
       <c r="N412" t="s">
-        <v>427</v>
+        <v>596</v>
       </c>
     </row>
     <row r="414" spans="1:14">
       <c r="A414" s="7" t="s">
-        <v>4928</v>
+        <v>4926</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>3227</v>
+        <v>3232</v>
       </c>
       <c r="C414" s="8" t="s">
-        <v>3228</v>
+        <v>3233</v>
       </c>
       <c r="D414" s="8" t="s">
-        <v>3229</v>
+        <v>3234</v>
       </c>
       <c r="E414" s="8" t="s">
         <v>30</v>
@@ -90931,24 +90934,24 @@
         <v>18</v>
       </c>
       <c r="M414" t="s">
-        <v>4929</v>
+        <v>2138</v>
       </c>
       <c r="N414" t="s">
-        <v>596</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="416" spans="1:14">
       <c r="A416" s="7" t="s">
-        <v>4930</v>
+        <v>4927</v>
       </c>
       <c r="B416" s="7" t="s">
-        <v>3232</v>
+        <v>3237</v>
       </c>
       <c r="C416" s="8" t="s">
-        <v>3233</v>
+        <v>3238</v>
       </c>
       <c r="D416" s="8" t="s">
-        <v>3234</v>
+        <v>3239</v>
       </c>
       <c r="E416" s="8" t="s">
         <v>30</v>
@@ -90966,7 +90969,7 @@
         <v>4668</v>
       </c>
       <c r="J416" s="8" t="s">
-        <v>4671</v>
+        <v>4708</v>
       </c>
       <c r="K416" t="s">
         <v>4669</v>
@@ -90975,24 +90978,24 @@
         <v>18</v>
       </c>
       <c r="M416" t="s">
-        <v>2138</v>
+        <v>3240</v>
       </c>
       <c r="N416" t="s">
-        <v>1063</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="418" spans="1:14">
       <c r="A418" s="7" t="s">
-        <v>4931</v>
+        <v>4928</v>
       </c>
       <c r="B418" s="7" t="s">
-        <v>3237</v>
+        <v>3254</v>
       </c>
       <c r="C418" s="8" t="s">
-        <v>3238</v>
+        <v>3255</v>
       </c>
       <c r="D418" s="8" t="s">
-        <v>3239</v>
+        <v>3256</v>
       </c>
       <c r="E418" s="8" t="s">
         <v>30</v>
@@ -91010,7 +91013,7 @@
         <v>4668</v>
       </c>
       <c r="J418" s="8" t="s">
-        <v>4708</v>
+        <v>4671</v>
       </c>
       <c r="K418" t="s">
         <v>4669</v>
@@ -91019,24 +91022,24 @@
         <v>18</v>
       </c>
       <c r="M418" t="s">
-        <v>3240</v>
+        <v>2833</v>
       </c>
       <c r="N418" t="s">
-        <v>3241</v>
+        <v>527</v>
       </c>
     </row>
     <row r="420" spans="1:14">
       <c r="A420" s="7" t="s">
-        <v>4932</v>
+        <v>4929</v>
       </c>
       <c r="B420" s="7" t="s">
-        <v>3254</v>
+        <v>3290</v>
       </c>
       <c r="C420" s="8" t="s">
-        <v>3255</v>
+        <v>368</v>
       </c>
       <c r="D420" s="8" t="s">
-        <v>3256</v>
+        <v>3291</v>
       </c>
       <c r="E420" s="8" t="s">
         <v>30</v>
@@ -91054,7 +91057,7 @@
         <v>4668</v>
       </c>
       <c r="J420" s="8" t="s">
-        <v>4671</v>
+        <v>4708</v>
       </c>
       <c r="K420" t="s">
         <v>4669</v>
@@ -91063,24 +91066,24 @@
         <v>18</v>
       </c>
       <c r="M420" t="s">
-        <v>2833</v>
+        <v>1585</v>
       </c>
       <c r="N420" t="s">
-        <v>527</v>
+        <v>405</v>
       </c>
     </row>
     <row r="422" spans="1:14">
       <c r="A422" s="7" t="s">
-        <v>4933</v>
+        <v>4930</v>
       </c>
       <c r="B422" s="7" t="s">
-        <v>3290</v>
+        <v>3293</v>
       </c>
       <c r="C422" s="8" t="s">
-        <v>368</v>
+        <v>2165</v>
       </c>
       <c r="D422" s="8" t="s">
-        <v>3291</v>
+        <v>3294</v>
       </c>
       <c r="E422" s="8" t="s">
         <v>30</v>
@@ -91098,7 +91101,7 @@
         <v>4668</v>
       </c>
       <c r="J422" s="8" t="s">
-        <v>4708</v>
+        <v>4671</v>
       </c>
       <c r="K422" t="s">
         <v>4669</v>
@@ -91107,24 +91110,24 @@
         <v>18</v>
       </c>
       <c r="M422" t="s">
-        <v>1585</v>
+        <v>4931</v>
       </c>
       <c r="N422" t="s">
-        <v>405</v>
+        <v>200</v>
       </c>
     </row>
     <row r="424" spans="1:14">
       <c r="A424" s="7" t="s">
-        <v>4934</v>
+        <v>4932</v>
       </c>
       <c r="B424" s="7" t="s">
-        <v>3293</v>
+        <v>3304</v>
       </c>
       <c r="C424" s="8" t="s">
-        <v>2165</v>
+        <v>3305</v>
       </c>
       <c r="D424" s="8" t="s">
-        <v>3294</v>
+        <v>3306</v>
       </c>
       <c r="E424" s="8" t="s">
         <v>30</v>
@@ -91151,24 +91154,24 @@
         <v>18</v>
       </c>
       <c r="M424" t="s">
-        <v>4935</v>
+        <v>4933</v>
       </c>
       <c r="N424" t="s">
-        <v>200</v>
+        <v>527</v>
       </c>
     </row>
     <row r="426" spans="1:14">
       <c r="A426" s="7" t="s">
-        <v>4936</v>
+        <v>4934</v>
       </c>
       <c r="B426" s="7" t="s">
-        <v>3304</v>
+        <v>3321</v>
       </c>
       <c r="C426" s="8" t="s">
-        <v>3305</v>
+        <v>2187</v>
       </c>
       <c r="D426" s="8" t="s">
-        <v>3306</v>
+        <v>3322</v>
       </c>
       <c r="E426" s="8" t="s">
         <v>30</v>
@@ -91185,9 +91188,6 @@
       <c r="I426" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J426" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K426" t="s">
         <v>4669</v>
       </c>
@@ -91195,24 +91195,24 @@
         <v>18</v>
       </c>
       <c r="M426" t="s">
-        <v>4937</v>
+        <v>4935</v>
       </c>
       <c r="N426" t="s">
-        <v>527</v>
+        <v>591</v>
       </c>
     </row>
     <row r="428" spans="1:14">
       <c r="A428" s="7" t="s">
-        <v>4938</v>
+        <v>4936</v>
       </c>
       <c r="B428" s="7" t="s">
-        <v>3321</v>
+        <v>3352</v>
       </c>
       <c r="C428" s="8" t="s">
-        <v>2187</v>
+        <v>391</v>
       </c>
       <c r="D428" s="8" t="s">
-        <v>3322</v>
+        <v>31</v>
       </c>
       <c r="E428" s="8" t="s">
         <v>30</v>
@@ -91236,21 +91236,21 @@
         <v>18</v>
       </c>
       <c r="M428" t="s">
-        <v>4939</v>
+        <v>1167</v>
       </c>
       <c r="N428" t="s">
-        <v>591</v>
+        <v>387</v>
       </c>
     </row>
     <row r="430" spans="1:14">
       <c r="A430" s="7" t="s">
-        <v>4940</v>
+        <v>4937</v>
       </c>
       <c r="B430" s="7" t="s">
-        <v>3352</v>
+        <v>3342</v>
       </c>
       <c r="C430" s="8" t="s">
-        <v>391</v>
+        <v>3343</v>
       </c>
       <c r="D430" s="8" t="s">
         <v>31</v>
@@ -91270,6 +91270,9 @@
       <c r="I430" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J430" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K430" t="s">
         <v>4669</v>
       </c>
@@ -91277,24 +91280,24 @@
         <v>18</v>
       </c>
       <c r="M430" t="s">
-        <v>1167</v>
+        <v>501</v>
       </c>
       <c r="N430" t="s">
-        <v>387</v>
+        <v>4938</v>
       </c>
     </row>
     <row r="432" spans="1:14">
       <c r="A432" s="7" t="s">
-        <v>4941</v>
+        <v>4939</v>
       </c>
       <c r="B432" s="7" t="s">
-        <v>3342</v>
+        <v>3373</v>
       </c>
       <c r="C432" s="8" t="s">
-        <v>3343</v>
+        <v>88</v>
       </c>
       <c r="D432" s="8" t="s">
-        <v>31</v>
+        <v>3374</v>
       </c>
       <c r="E432" s="8" t="s">
         <v>30</v>
@@ -91311,9 +91314,6 @@
       <c r="I432" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J432" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K432" t="s">
         <v>4669</v>
       </c>
@@ -91321,24 +91321,24 @@
         <v>18</v>
       </c>
       <c r="M432" t="s">
-        <v>501</v>
+        <v>3375</v>
       </c>
       <c r="N432" t="s">
-        <v>4942</v>
+        <v>565</v>
       </c>
     </row>
     <row r="434" spans="1:14">
       <c r="A434" s="7" t="s">
-        <v>4943</v>
+        <v>4940</v>
       </c>
       <c r="B434" s="7" t="s">
-        <v>3373</v>
+        <v>3377</v>
       </c>
       <c r="C434" s="8" t="s">
-        <v>88</v>
+        <v>3378</v>
       </c>
       <c r="D434" s="8" t="s">
-        <v>3374</v>
+        <v>3379</v>
       </c>
       <c r="E434" s="8" t="s">
         <v>30</v>
@@ -91362,24 +91362,24 @@
         <v>18</v>
       </c>
       <c r="M434" t="s">
-        <v>3375</v>
+        <v>452</v>
       </c>
       <c r="N434" t="s">
-        <v>565</v>
+        <v>35</v>
       </c>
     </row>
     <row r="436" spans="1:14">
       <c r="A436" s="7" t="s">
-        <v>4944</v>
+        <v>4941</v>
       </c>
       <c r="B436" s="7" t="s">
-        <v>3377</v>
+        <v>3389</v>
       </c>
       <c r="C436" s="8" t="s">
-        <v>3378</v>
+        <v>3390</v>
       </c>
       <c r="D436" s="8" t="s">
-        <v>3379</v>
+        <v>3391</v>
       </c>
       <c r="E436" s="8" t="s">
         <v>30</v>
@@ -91403,24 +91403,24 @@
         <v>18</v>
       </c>
       <c r="M436" t="s">
-        <v>452</v>
+        <v>4639</v>
       </c>
       <c r="N436" t="s">
-        <v>35</v>
+        <v>395</v>
       </c>
     </row>
     <row r="438" spans="1:14">
       <c r="A438" s="7" t="s">
-        <v>4945</v>
+        <v>4942</v>
       </c>
       <c r="B438" s="7" t="s">
-        <v>3389</v>
+        <v>3397</v>
       </c>
       <c r="C438" s="8" t="s">
-        <v>3390</v>
+        <v>1392</v>
       </c>
       <c r="D438" s="8" t="s">
-        <v>3391</v>
+        <v>3395</v>
       </c>
       <c r="E438" s="8" t="s">
         <v>30</v>
@@ -91444,21 +91444,21 @@
         <v>18</v>
       </c>
       <c r="M438" t="s">
-        <v>4639</v>
+        <v>1933</v>
       </c>
       <c r="N438" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="440" spans="1:14">
       <c r="A440" s="7" t="s">
-        <v>4946</v>
+        <v>4943</v>
       </c>
       <c r="B440" s="7" t="s">
-        <v>3397</v>
+        <v>3393</v>
       </c>
       <c r="C440" s="8" t="s">
-        <v>1392</v>
+        <v>3394</v>
       </c>
       <c r="D440" s="8" t="s">
         <v>3395</v>
@@ -91493,16 +91493,16 @@
     </row>
     <row r="442" spans="1:14">
       <c r="A442" s="7" t="s">
-        <v>4947</v>
+        <v>4944</v>
       </c>
       <c r="B442" s="7" t="s">
-        <v>3393</v>
+        <v>3420</v>
       </c>
       <c r="C442" s="8" t="s">
-        <v>3394</v>
+        <v>3421</v>
       </c>
       <c r="D442" s="8" t="s">
-        <v>3395</v>
+        <v>3422</v>
       </c>
       <c r="E442" s="8" t="s">
         <v>30</v>
@@ -91519,6 +91519,9 @@
       <c r="I442" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J442" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K442" t="s">
         <v>4669</v>
       </c>
@@ -91526,24 +91529,24 @@
         <v>18</v>
       </c>
       <c r="M442" t="s">
-        <v>1933</v>
+        <v>1216</v>
       </c>
       <c r="N442" t="s">
-        <v>405</v>
+        <v>427</v>
       </c>
     </row>
     <row r="444" spans="1:14">
       <c r="A444" s="7" t="s">
-        <v>4948</v>
+        <v>4945</v>
       </c>
       <c r="B444" s="7" t="s">
-        <v>3420</v>
+        <v>3429</v>
       </c>
       <c r="C444" s="8" t="s">
-        <v>3421</v>
+        <v>3430</v>
       </c>
       <c r="D444" s="8" t="s">
-        <v>3422</v>
+        <v>1601</v>
       </c>
       <c r="E444" s="8" t="s">
         <v>30</v>
@@ -91560,9 +91563,6 @@
       <c r="I444" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J444" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K444" t="s">
         <v>4669</v>
       </c>
@@ -91570,24 +91570,24 @@
         <v>18</v>
       </c>
       <c r="M444" t="s">
-        <v>1216</v>
+        <v>3431</v>
       </c>
       <c r="N444" t="s">
-        <v>427</v>
+        <v>601</v>
       </c>
     </row>
     <row r="446" spans="1:14">
       <c r="A446" s="7" t="s">
-        <v>4949</v>
+        <v>4946</v>
       </c>
       <c r="B446" s="7" t="s">
-        <v>3429</v>
+        <v>4947</v>
       </c>
       <c r="C446" s="8" t="s">
-        <v>3430</v>
+        <v>3143</v>
       </c>
       <c r="D446" s="8" t="s">
-        <v>1601</v>
+        <v>3448</v>
       </c>
       <c r="E446" s="8" t="s">
         <v>30</v>
@@ -91604,6 +91604,9 @@
       <c r="I446" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J446" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K446" t="s">
         <v>4669</v>
       </c>
@@ -91611,21 +91614,21 @@
         <v>18</v>
       </c>
       <c r="M446" t="s">
-        <v>3431</v>
+        <v>1362</v>
       </c>
       <c r="N446" t="s">
-        <v>601</v>
+        <v>27</v>
       </c>
     </row>
     <row r="448" spans="1:14">
       <c r="A448" s="7" t="s">
-        <v>4950</v>
+        <v>4948</v>
       </c>
       <c r="B448" s="7" t="s">
-        <v>4951</v>
+        <v>3446</v>
       </c>
       <c r="C448" s="8" t="s">
-        <v>3143</v>
+        <v>3447</v>
       </c>
       <c r="D448" s="8" t="s">
         <v>3448</v>
@@ -91655,7 +91658,7 @@
         <v>18</v>
       </c>
       <c r="M448" t="s">
-        <v>1362</v>
+        <v>2633</v>
       </c>
       <c r="N448" t="s">
         <v>27</v>
@@ -91663,16 +91666,16 @@
     </row>
     <row r="450" spans="1:16">
       <c r="A450" s="7" t="s">
-        <v>4952</v>
+        <v>4949</v>
       </c>
       <c r="B450" s="7" t="s">
-        <v>3446</v>
+        <v>3515</v>
       </c>
       <c r="C450" s="8" t="s">
-        <v>3447</v>
+        <v>3516</v>
       </c>
       <c r="D450" s="8" t="s">
-        <v>3448</v>
+        <v>3517</v>
       </c>
       <c r="E450" s="8" t="s">
         <v>30</v>
@@ -91699,21 +91702,21 @@
         <v>18</v>
       </c>
       <c r="M450" t="s">
-        <v>2633</v>
+        <v>3518</v>
       </c>
       <c r="N450" t="s">
-        <v>27</v>
+        <v>427</v>
       </c>
     </row>
     <row r="452" spans="1:16">
       <c r="A452" s="7" t="s">
-        <v>4953</v>
+        <v>4950</v>
       </c>
       <c r="B452" s="7" t="s">
-        <v>3515</v>
+        <v>4951</v>
       </c>
       <c r="C452" s="8" t="s">
-        <v>3516</v>
+        <v>4952</v>
       </c>
       <c r="D452" s="8" t="s">
         <v>3517</v>
@@ -91734,7 +91737,7 @@
         <v>4668</v>
       </c>
       <c r="J452" s="8" t="s">
-        <v>4671</v>
+        <v>4716</v>
       </c>
       <c r="K452" t="s">
         <v>4669</v>
@@ -91743,21 +91746,21 @@
         <v>18</v>
       </c>
       <c r="M452" t="s">
-        <v>3518</v>
+        <v>3026</v>
       </c>
       <c r="N452" t="s">
-        <v>427</v>
+        <v>254</v>
       </c>
     </row>
     <row r="454" spans="1:16">
       <c r="A454" s="7" t="s">
+        <v>4953</v>
+      </c>
+      <c r="B454" s="7" t="s">
         <v>4954</v>
       </c>
-      <c r="B454" s="7" t="s">
+      <c r="C454" s="8" t="s">
         <v>4955</v>
-      </c>
-      <c r="C454" s="8" t="s">
-        <v>4956</v>
       </c>
       <c r="D454" s="8" t="s">
         <v>3517</v>
@@ -91795,13 +91798,13 @@
     </row>
     <row r="456" spans="1:16">
       <c r="A456" s="7" t="s">
+        <v>4956</v>
+      </c>
+      <c r="B456" s="7" t="s">
         <v>4957</v>
       </c>
-      <c r="B456" s="7" t="s">
+      <c r="C456" s="8" t="s">
         <v>4958</v>
-      </c>
-      <c r="C456" s="8" t="s">
-        <v>4959</v>
       </c>
       <c r="D456" s="8" t="s">
         <v>3517</v>
@@ -91839,13 +91842,13 @@
     </row>
     <row r="458" spans="1:16">
       <c r="A458" s="7" t="s">
-        <v>4960</v>
+        <v>4959</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>4961</v>
+        <v>3523</v>
       </c>
       <c r="C458" s="8" t="s">
-        <v>4962</v>
+        <v>3524</v>
       </c>
       <c r="D458" s="8" t="s">
         <v>3517</v>
@@ -91866,7 +91869,7 @@
         <v>4668</v>
       </c>
       <c r="J458" s="8" t="s">
-        <v>4716</v>
+        <v>4671</v>
       </c>
       <c r="K458" t="s">
         <v>4669</v>
@@ -91875,7 +91878,7 @@
         <v>18</v>
       </c>
       <c r="M458" t="s">
-        <v>3026</v>
+        <v>941</v>
       </c>
       <c r="N458" t="s">
         <v>254</v>
@@ -91883,13 +91886,13 @@
     </row>
     <row r="460" spans="1:16">
       <c r="A460" s="7" t="s">
-        <v>4963</v>
+        <v>4960</v>
       </c>
       <c r="B460" s="7" t="s">
-        <v>3523</v>
+        <v>4961</v>
       </c>
       <c r="C460" s="8" t="s">
-        <v>3524</v>
+        <v>3798</v>
       </c>
       <c r="D460" s="8" t="s">
         <v>3517</v>
@@ -91927,13 +91930,13 @@
     </row>
     <row r="462" spans="1:16">
       <c r="A462" s="7" t="s">
-        <v>4964</v>
+        <v>4962</v>
       </c>
       <c r="B462" s="7" t="s">
-        <v>4965</v>
+        <v>3520</v>
       </c>
       <c r="C462" s="8" t="s">
-        <v>3798</v>
+        <v>3521</v>
       </c>
       <c r="D462" s="8" t="s">
         <v>3517</v>
@@ -91960,27 +91963,30 @@
         <v>4669</v>
       </c>
       <c r="L462" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="M462" t="s">
-        <v>941</v>
+        <v>3213</v>
       </c>
       <c r="N462" t="s">
-        <v>254</v>
+        <v>427</v>
+      </c>
+      <c r="P462" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="464" spans="1:16">
       <c r="A464" s="7" t="s">
-        <v>4966</v>
+        <v>4963</v>
       </c>
       <c r="B464" s="7" t="s">
-        <v>3520</v>
+        <v>3539</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>3521</v>
+        <v>1013</v>
       </c>
       <c r="D464" s="8" t="s">
-        <v>3517</v>
+        <v>3540</v>
       </c>
       <c r="E464" s="8" t="s">
         <v>30</v>
@@ -91997,37 +92003,31 @@
       <c r="I464" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J464" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K464" t="s">
         <v>4669</v>
       </c>
       <c r="L464" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="M464" t="s">
-        <v>3213</v>
+        <v>3541</v>
       </c>
       <c r="N464" t="s">
-        <v>427</v>
-      </c>
-      <c r="P464" t="s">
-        <v>339</v>
+        <v>551</v>
       </c>
     </row>
     <row r="466" spans="1:14">
       <c r="A466" s="7" t="s">
-        <v>4967</v>
+        <v>4964</v>
       </c>
       <c r="B466" s="7" t="s">
-        <v>3539</v>
+        <v>3543</v>
       </c>
       <c r="C466" s="8" t="s">
-        <v>1013</v>
+        <v>3544</v>
       </c>
       <c r="D466" s="8" t="s">
-        <v>3540</v>
+        <v>3545</v>
       </c>
       <c r="E466" s="8" t="s">
         <v>30</v>
@@ -92044,6 +92044,9 @@
       <c r="I466" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J466" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K466" t="s">
         <v>4669</v>
       </c>
@@ -92051,24 +92054,24 @@
         <v>18</v>
       </c>
       <c r="M466" t="s">
-        <v>3541</v>
+        <v>4029</v>
       </c>
       <c r="N466" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
     </row>
     <row r="468" spans="1:14">
       <c r="A468" s="7" t="s">
-        <v>4968</v>
+        <v>4965</v>
       </c>
       <c r="B468" s="7" t="s">
-        <v>3543</v>
+        <v>3595</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>3544</v>
+        <v>391</v>
       </c>
       <c r="D468" s="8" t="s">
-        <v>3545</v>
+        <v>3596</v>
       </c>
       <c r="E468" s="8" t="s">
         <v>30</v>
@@ -92085,9 +92088,6 @@
       <c r="I468" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J468" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K468" t="s">
         <v>4669</v>
       </c>
@@ -92095,24 +92095,24 @@
         <v>18</v>
       </c>
       <c r="M468" t="s">
-        <v>4029</v>
+        <v>1886</v>
       </c>
       <c r="N468" t="s">
-        <v>527</v>
+        <v>365</v>
       </c>
     </row>
     <row r="470" spans="1:14">
       <c r="A470" s="7" t="s">
-        <v>4969</v>
+        <v>4966</v>
       </c>
       <c r="B470" s="7" t="s">
-        <v>3595</v>
+        <v>3599</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>391</v>
+        <v>2315</v>
       </c>
       <c r="D470" s="8" t="s">
-        <v>3596</v>
+        <v>3600</v>
       </c>
       <c r="E470" s="8" t="s">
         <v>30</v>
@@ -92129,6 +92129,9 @@
       <c r="I470" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J470" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K470" t="s">
         <v>4669</v>
       </c>
@@ -92136,24 +92139,24 @@
         <v>18</v>
       </c>
       <c r="M470" t="s">
-        <v>1886</v>
+        <v>2121</v>
       </c>
       <c r="N470" t="s">
-        <v>365</v>
+        <v>672</v>
       </c>
     </row>
     <row r="472" spans="1:14">
       <c r="A472" s="7" t="s">
-        <v>4970</v>
+        <v>4967</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>3599</v>
+        <v>3603</v>
       </c>
       <c r="C472" s="8" t="s">
-        <v>2315</v>
+        <v>3604</v>
       </c>
       <c r="D472" s="8" t="s">
-        <v>3600</v>
+        <v>3605</v>
       </c>
       <c r="E472" s="8" t="s">
         <v>30</v>
@@ -92170,9 +92173,6 @@
       <c r="I472" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J472" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K472" t="s">
         <v>4669</v>
       </c>
@@ -92180,24 +92180,24 @@
         <v>18</v>
       </c>
       <c r="M472" t="s">
-        <v>2121</v>
+        <v>1381</v>
       </c>
       <c r="N472" t="s">
-        <v>672</v>
+        <v>387</v>
       </c>
     </row>
     <row r="474" spans="1:14">
       <c r="A474" s="7" t="s">
-        <v>4971</v>
+        <v>4968</v>
       </c>
       <c r="B474" s="7" t="s">
-        <v>3603</v>
+        <v>3614</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>3604</v>
+        <v>245</v>
       </c>
       <c r="D474" s="8" t="s">
-        <v>3605</v>
+        <v>3615</v>
       </c>
       <c r="E474" s="8" t="s">
         <v>30</v>
@@ -92214,6 +92214,9 @@
       <c r="I474" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J474" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K474" t="s">
         <v>4669</v>
       </c>
@@ -92221,24 +92224,24 @@
         <v>18</v>
       </c>
       <c r="M474" t="s">
-        <v>1381</v>
+        <v>199</v>
       </c>
       <c r="N474" t="s">
-        <v>387</v>
+        <v>200</v>
       </c>
     </row>
     <row r="476" spans="1:14">
       <c r="A476" s="7" t="s">
-        <v>4972</v>
+        <v>4969</v>
       </c>
       <c r="B476" s="7" t="s">
-        <v>3614</v>
+        <v>3617</v>
       </c>
       <c r="C476" s="8" t="s">
-        <v>245</v>
+        <v>1181</v>
       </c>
       <c r="D476" s="8" t="s">
-        <v>3615</v>
+        <v>3618</v>
       </c>
       <c r="E476" s="8" t="s">
         <v>30</v>
@@ -92262,27 +92265,27 @@
         <v>4669</v>
       </c>
       <c r="L476" t="s">
-        <v>18</v>
+        <v>1453</v>
       </c>
       <c r="M476" t="s">
-        <v>199</v>
+        <v>314</v>
       </c>
       <c r="N476" t="s">
-        <v>200</v>
+        <v>381</v>
       </c>
     </row>
     <row r="478" spans="1:14">
       <c r="A478" s="7" t="s">
-        <v>4973</v>
+        <v>4970</v>
       </c>
       <c r="B478" s="7" t="s">
-        <v>3617</v>
+        <v>4971</v>
       </c>
       <c r="C478" s="8" t="s">
-        <v>1181</v>
+        <v>1426</v>
       </c>
       <c r="D478" s="8" t="s">
-        <v>3618</v>
+        <v>3703</v>
       </c>
       <c r="E478" s="8" t="s">
         <v>30</v>
@@ -92299,31 +92302,28 @@
       <c r="I478" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J478" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K478" t="s">
         <v>4669</v>
       </c>
       <c r="L478" t="s">
-        <v>1453</v>
+        <v>18</v>
       </c>
       <c r="M478" t="s">
-        <v>314</v>
+        <v>1167</v>
       </c>
       <c r="N478" t="s">
-        <v>381</v>
+        <v>541</v>
       </c>
     </row>
     <row r="480" spans="1:14">
       <c r="A480" s="7" t="s">
-        <v>4974</v>
+        <v>4972</v>
       </c>
       <c r="B480" s="7" t="s">
-        <v>4975</v>
+        <v>3702</v>
       </c>
       <c r="C480" s="8" t="s">
-        <v>1426</v>
+        <v>1392</v>
       </c>
       <c r="D480" s="8" t="s">
         <v>3703</v>
@@ -92350,7 +92350,7 @@
         <v>18</v>
       </c>
       <c r="M480" t="s">
-        <v>1167</v>
+        <v>1212</v>
       </c>
       <c r="N480" t="s">
         <v>541</v>
@@ -92358,16 +92358,16 @@
     </row>
     <row r="482" spans="1:14">
       <c r="A482" s="7" t="s">
-        <v>4976</v>
+        <v>4973</v>
       </c>
       <c r="B482" s="7" t="s">
-        <v>3702</v>
+        <v>3722</v>
       </c>
       <c r="C482" s="8" t="s">
-        <v>1392</v>
+        <v>1148</v>
       </c>
       <c r="D482" s="8" t="s">
-        <v>3703</v>
+        <v>3723</v>
       </c>
       <c r="E482" s="8" t="s">
         <v>30</v>
@@ -92384,6 +92384,9 @@
       <c r="I482" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J482" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K482" t="s">
         <v>4669</v>
       </c>
@@ -92391,24 +92394,24 @@
         <v>18</v>
       </c>
       <c r="M482" t="s">
-        <v>1212</v>
+        <v>3135</v>
       </c>
       <c r="N482" t="s">
-        <v>541</v>
+        <v>596</v>
       </c>
     </row>
     <row r="484" spans="1:14">
       <c r="A484" s="7" t="s">
-        <v>4977</v>
+        <v>4974</v>
       </c>
       <c r="B484" s="7" t="s">
-        <v>3722</v>
+        <v>3740</v>
       </c>
       <c r="C484" s="8" t="s">
-        <v>1148</v>
+        <v>3741</v>
       </c>
       <c r="D484" s="8" t="s">
-        <v>3723</v>
+        <v>3726</v>
       </c>
       <c r="E484" s="8" t="s">
         <v>30</v>
@@ -92435,21 +92438,21 @@
         <v>18</v>
       </c>
       <c r="M484" t="s">
-        <v>3135</v>
+        <v>418</v>
       </c>
       <c r="N484" t="s">
-        <v>596</v>
+        <v>412</v>
       </c>
     </row>
     <row r="486" spans="1:14">
       <c r="A486" s="7" t="s">
-        <v>4978</v>
+        <v>4975</v>
       </c>
       <c r="B486" s="7" t="s">
-        <v>3740</v>
+        <v>3728</v>
       </c>
       <c r="C486" s="8" t="s">
-        <v>3741</v>
+        <v>65</v>
       </c>
       <c r="D486" s="8" t="s">
         <v>3726</v>
@@ -92469,9 +92472,6 @@
       <c r="I486" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J486" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K486" t="s">
         <v>4669</v>
       </c>
@@ -92479,21 +92479,21 @@
         <v>18</v>
       </c>
       <c r="M486" t="s">
-        <v>418</v>
+        <v>3714</v>
       </c>
       <c r="N486" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
     </row>
     <row r="488" spans="1:14">
       <c r="A488" s="7" t="s">
-        <v>4979</v>
+        <v>4976</v>
       </c>
       <c r="B488" s="7" t="s">
-        <v>3728</v>
+        <v>3730</v>
       </c>
       <c r="C488" s="8" t="s">
-        <v>65</v>
+        <v>3731</v>
       </c>
       <c r="D488" s="8" t="s">
         <v>3726</v>
@@ -92520,24 +92520,24 @@
         <v>18</v>
       </c>
       <c r="M488" t="s">
-        <v>3714</v>
+        <v>1230</v>
       </c>
       <c r="N488" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="490" spans="1:14">
       <c r="A490" s="7" t="s">
-        <v>4980</v>
+        <v>4977</v>
       </c>
       <c r="B490" s="7" t="s">
-        <v>3730</v>
+        <v>3761</v>
       </c>
       <c r="C490" s="8" t="s">
-        <v>3731</v>
+        <v>3762</v>
       </c>
       <c r="D490" s="8" t="s">
-        <v>3726</v>
+        <v>3756</v>
       </c>
       <c r="E490" s="8" t="s">
         <v>30</v>
@@ -92561,7 +92561,7 @@
         <v>18</v>
       </c>
       <c r="M490" t="s">
-        <v>1230</v>
+        <v>1914</v>
       </c>
       <c r="N490" t="s">
         <v>380</v>
@@ -92569,16 +92569,16 @@
     </row>
     <row r="492" spans="1:14">
       <c r="A492" s="7" t="s">
+        <v>4978</v>
+      </c>
+      <c r="B492" s="7" t="s">
+        <v>4979</v>
+      </c>
+      <c r="C492" s="8" t="s">
+        <v>4980</v>
+      </c>
+      <c r="D492" s="8" t="s">
         <v>4981</v>
-      </c>
-      <c r="B492" s="7" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C492" s="8" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D492" s="8" t="s">
-        <v>3756</v>
       </c>
       <c r="E492" s="8" t="s">
         <v>30</v>
@@ -92595,17 +92595,20 @@
       <c r="I492" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J492" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K492" t="s">
         <v>4669</v>
       </c>
       <c r="L492" t="s">
-        <v>18</v>
+        <v>1453</v>
       </c>
       <c r="M492" t="s">
-        <v>1914</v>
+        <v>247</v>
       </c>
       <c r="N492" t="s">
-        <v>380</v>
+        <v>35</v>
       </c>
     </row>
     <row r="494" spans="1:14">
@@ -92619,7 +92622,7 @@
         <v>4984</v>
       </c>
       <c r="D494" s="8" t="s">
-        <v>4985</v>
+        <v>3769</v>
       </c>
       <c r="E494" s="8" t="s">
         <v>30</v>
@@ -92643,27 +92646,27 @@
         <v>4669</v>
       </c>
       <c r="L494" t="s">
-        <v>1453</v>
+        <v>18</v>
       </c>
       <c r="M494" t="s">
-        <v>247</v>
+        <v>550</v>
       </c>
       <c r="N494" t="s">
-        <v>35</v>
+        <v>601</v>
       </c>
     </row>
     <row r="496" spans="1:14">
       <c r="A496" s="7" t="s">
-        <v>4986</v>
+        <v>4985</v>
       </c>
       <c r="B496" s="7" t="s">
-        <v>4987</v>
+        <v>3786</v>
       </c>
       <c r="C496" s="8" t="s">
-        <v>4988</v>
+        <v>3787</v>
       </c>
       <c r="D496" s="8" t="s">
-        <v>3769</v>
+        <v>3788</v>
       </c>
       <c r="E496" s="8" t="s">
         <v>30</v>
@@ -92690,7 +92693,7 @@
         <v>18</v>
       </c>
       <c r="M496" t="s">
-        <v>550</v>
+        <v>4986</v>
       </c>
       <c r="N496" t="s">
         <v>601</v>
@@ -92698,16 +92701,16 @@
     </row>
     <row r="498" spans="1:16">
       <c r="A498" s="7" t="s">
-        <v>4989</v>
+        <v>4987</v>
       </c>
       <c r="B498" s="7" t="s">
-        <v>3786</v>
+        <v>3795</v>
       </c>
       <c r="C498" s="8" t="s">
-        <v>3787</v>
+        <v>88</v>
       </c>
       <c r="D498" s="8" t="s">
-        <v>3788</v>
+        <v>3791</v>
       </c>
       <c r="E498" s="8" t="s">
         <v>30</v>
@@ -92724,9 +92727,6 @@
       <c r="I498" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J498" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K498" t="s">
         <v>4669</v>
       </c>
@@ -92734,21 +92734,21 @@
         <v>18</v>
       </c>
       <c r="M498" t="s">
-        <v>4990</v>
+        <v>3792</v>
       </c>
       <c r="N498" t="s">
-        <v>601</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="500" spans="1:16">
       <c r="A500" s="7" t="s">
-        <v>4991</v>
+        <v>4988</v>
       </c>
       <c r="B500" s="7" t="s">
-        <v>3795</v>
+        <v>3790</v>
       </c>
       <c r="C500" s="8" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="D500" s="8" t="s">
         <v>3791</v>
@@ -92772,27 +92772,33 @@
         <v>4669</v>
       </c>
       <c r="L500" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="M500" t="s">
         <v>3792</v>
       </c>
       <c r="N500" t="s">
-        <v>3475</v>
+        <v>531</v>
+      </c>
+      <c r="O500" t="s">
+        <v>584</v>
+      </c>
+      <c r="P500" t="s">
+        <v>3710</v>
       </c>
     </row>
     <row r="502" spans="1:16">
       <c r="A502" s="7" t="s">
-        <v>4992</v>
+        <v>4989</v>
       </c>
       <c r="B502" s="7" t="s">
-        <v>3790</v>
+        <v>3809</v>
       </c>
       <c r="C502" s="8" t="s">
-        <v>179</v>
+        <v>1392</v>
       </c>
       <c r="D502" s="8" t="s">
-        <v>3791</v>
+        <v>3810</v>
       </c>
       <c r="E502" s="8" t="s">
         <v>30</v>
@@ -92813,33 +92819,27 @@
         <v>4669</v>
       </c>
       <c r="L502" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="M502" t="s">
-        <v>3792</v>
+        <v>386</v>
       </c>
       <c r="N502" t="s">
-        <v>531</v>
-      </c>
-      <c r="O502" t="s">
-        <v>584</v>
-      </c>
-      <c r="P502" t="s">
-        <v>3710</v>
+        <v>380</v>
       </c>
     </row>
     <row r="504" spans="1:16">
       <c r="A504" s="7" t="s">
-        <v>4993</v>
+        <v>4990</v>
       </c>
       <c r="B504" s="7" t="s">
-        <v>3809</v>
+        <v>3840</v>
       </c>
       <c r="C504" s="8" t="s">
-        <v>1392</v>
+        <v>319</v>
       </c>
       <c r="D504" s="8" t="s">
-        <v>3810</v>
+        <v>3841</v>
       </c>
       <c r="E504" s="8" t="s">
         <v>30</v>
@@ -92856,6 +92856,9 @@
       <c r="I504" s="8" t="s">
         <v>4668</v>
       </c>
+      <c r="J504" s="8" t="s">
+        <v>4671</v>
+      </c>
       <c r="K504" t="s">
         <v>4669</v>
       </c>
@@ -92863,21 +92866,21 @@
         <v>18</v>
       </c>
       <c r="M504" t="s">
-        <v>386</v>
+        <v>2995</v>
       </c>
       <c r="N504" t="s">
-        <v>380</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="506" spans="1:16">
       <c r="A506" s="7" t="s">
-        <v>4994</v>
+        <v>4991</v>
       </c>
       <c r="B506" s="7" t="s">
-        <v>3840</v>
+        <v>3843</v>
       </c>
       <c r="C506" s="8" t="s">
-        <v>319</v>
+        <v>1219</v>
       </c>
       <c r="D506" s="8" t="s">
         <v>3841</v>
@@ -92897,9 +92900,6 @@
       <c r="I506" s="8" t="s">
         <v>4668</v>
       </c>
-      <c r="J506" s="8" t="s">
-        <v>4671</v>
-      </c>
       <c r="K506" t="s">
         <v>4669</v>
       </c>
@@ -92907,50 +92907,9 @@
         <v>18</v>
       </c>
       <c r="M506" t="s">
-        <v>2995</v>
+        <v>3302</v>
       </c>
       <c r="N506" t="s">
-        <v>4385</v>
-      </c>
-    </row>
-    <row r="508" spans="1:16">
-      <c r="A508" s="7" t="s">
-        <v>4995</v>
-      </c>
-      <c r="B508" s="7" t="s">
-        <v>3843</v>
-      </c>
-      <c r="C508" s="8" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D508" s="8" t="s">
-        <v>3841</v>
-      </c>
-      <c r="E508" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F508" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="G508" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H508" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="I508" s="8" t="s">
-        <v>4668</v>
-      </c>
-      <c r="K508" t="s">
-        <v>4669</v>
-      </c>
-      <c r="L508" t="s">
-        <v>18</v>
-      </c>
-      <c r="M508" t="s">
-        <v>3302</v>
-      </c>
-      <c r="N508" t="s">
         <v>607</v>
       </c>
     </row>
@@ -93260,10 +93219,10 @@
     <hyperlink ref="B300" r:id="rId302"/>
     <hyperlink ref="A302" r:id="rId303"/>
     <hyperlink ref="B302" r:id="rId304"/>
-    <hyperlink ref="A304" r:id="rId305"/>
-    <hyperlink ref="B304" r:id="rId306"/>
-    <hyperlink ref="A305" r:id="rId307"/>
-    <hyperlink ref="B305" r:id="rId308"/>
+    <hyperlink ref="A303" r:id="rId305"/>
+    <hyperlink ref="B303" r:id="rId306"/>
+    <hyperlink ref="A304" r:id="rId307"/>
+    <hyperlink ref="B304" r:id="rId308"/>
     <hyperlink ref="A306" r:id="rId309"/>
     <hyperlink ref="B306" r:id="rId310"/>
     <hyperlink ref="A308" r:id="rId311"/>
@@ -93466,8 +93425,6 @@
     <hyperlink ref="B504" r:id="rId508"/>
     <hyperlink ref="A506" r:id="rId509"/>
     <hyperlink ref="B506" r:id="rId510"/>
-    <hyperlink ref="A508" r:id="rId511"/>
-    <hyperlink ref="B508" r:id="rId512"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -93548,7 +93505,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
-        <v>4996</v>
+        <v>4992</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3849</v>
@@ -93572,10 +93529,10 @@
         <v>491</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K2" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -93589,7 +93546,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="7" t="s">
-        <v>4999</v>
+        <v>4995</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3870</v>
@@ -93613,10 +93570,10 @@
         <v>491</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K4" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
@@ -93630,7 +93587,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="7" t="s">
-        <v>5000</v>
+        <v>4996</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3943</v>
@@ -93654,16 +93611,16 @@
         <v>491</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>4993</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4994</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
         <v>4997</v>
-      </c>
-      <c r="K6" t="s">
-        <v>4998</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>5001</v>
       </c>
       <c r="N6" t="s">
         <v>427</v>
@@ -93671,16 +93628,16 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="7" t="s">
-        <v>5002</v>
+        <v>4998</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>5003</v>
+        <v>4999</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>5004</v>
+        <v>5000</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>5005</v>
+        <v>5001</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>30</v>
@@ -93695,10 +93652,10 @@
         <v>491</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K8" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L8" t="s">
         <v>18</v>
@@ -93712,7 +93669,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="7" t="s">
-        <v>5006</v>
+        <v>5002</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>4012</v>
@@ -93736,10 +93693,10 @@
         <v>491</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K10" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L10" t="s">
         <v>18</v>
@@ -93753,7 +93710,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="7" t="s">
-        <v>5007</v>
+        <v>5003</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>4149</v>
@@ -93777,10 +93734,10 @@
         <v>491</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K12" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L12" t="s">
         <v>1453</v>
@@ -93794,7 +93751,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="7" t="s">
-        <v>5008</v>
+        <v>5004</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4188</v>
@@ -93818,10 +93775,10 @@
         <v>491</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K14" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L14" t="s">
         <v>438</v>
@@ -93838,7 +93795,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="7" t="s">
-        <v>5009</v>
+        <v>5005</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>4201</v>
@@ -93862,10 +93819,10 @@
         <v>491</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K16" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L16" t="s">
         <v>438</v>
@@ -93877,12 +93834,12 @@
         <v>672</v>
       </c>
       <c r="P16" t="s">
-        <v>5010</v>
+        <v>5006</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="7" t="s">
-        <v>5011</v>
+        <v>5007</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>4280</v>
@@ -93906,10 +93863,10 @@
         <v>491</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K18" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L18" t="s">
         <v>18</v>
@@ -93923,7 +93880,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="7" t="s">
-        <v>5012</v>
+        <v>5008</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>4321</v>
@@ -93947,10 +93904,10 @@
         <v>491</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K20" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L20" t="s">
         <v>18</v>
@@ -93964,7 +93921,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="7" t="s">
-        <v>5013</v>
+        <v>5009</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>4349</v>
@@ -93988,10 +93945,10 @@
         <v>491</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K22" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L22" t="s">
         <v>18</v>
@@ -94005,7 +93962,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="7" t="s">
-        <v>5014</v>
+        <v>5010</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>4353</v>
@@ -94029,10 +93986,10 @@
         <v>491</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K24" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L24" t="s">
         <v>18</v>
@@ -94046,7 +94003,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="7" t="s">
-        <v>5015</v>
+        <v>5011</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>4378</v>
@@ -94073,7 +94030,7 @@
         <v>80</v>
       </c>
       <c r="K26" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L26" t="s">
         <v>18</v>
@@ -94087,7 +94044,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="7" t="s">
-        <v>5016</v>
+        <v>5012</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>4421</v>
@@ -94111,10 +94068,10 @@
         <v>491</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K28" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L28" t="s">
         <v>438</v>
@@ -94122,7 +94079,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="7" t="s">
-        <v>5017</v>
+        <v>5013</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>4474</v>
@@ -94146,10 +94103,10 @@
         <v>491</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K30" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L30" t="s">
         <v>18</v>
@@ -94163,7 +94120,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="7" t="s">
-        <v>5018</v>
+        <v>5014</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>4483</v>
@@ -94187,10 +94144,10 @@
         <v>491</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K32" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L32" t="s">
         <v>18</v>
@@ -94204,7 +94161,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="7" t="s">
-        <v>5019</v>
+        <v>5015</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>4501</v>
@@ -94228,10 +94185,10 @@
         <v>491</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K34" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L34" t="s">
         <v>18</v>
@@ -94245,7 +94202,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="7" t="s">
-        <v>5020</v>
+        <v>5016</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>4516</v>
@@ -94269,10 +94226,10 @@
         <v>491</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K36" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L36" t="s">
         <v>18</v>
@@ -94286,7 +94243,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="7" t="s">
-        <v>5021</v>
+        <v>5017</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>4511</v>
@@ -94310,10 +94267,10 @@
         <v>491</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K38" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L38" t="s">
         <v>18</v>
@@ -94327,7 +94284,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="7" t="s">
-        <v>5022</v>
+        <v>5018</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>4575</v>
@@ -94351,10 +94308,10 @@
         <v>491</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>4997</v>
+        <v>4993</v>
       </c>
       <c r="K40" t="s">
-        <v>4998</v>
+        <v>4994</v>
       </c>
       <c r="L40" t="s">
         <v>18</v>

</xml_diff>